<commit_message>
added ideas and stuff
</commit_message>
<xml_diff>
--- a/data/survey-serengeti-tiger-king.xlsx
+++ b/data/survey-serengeti-tiger-king.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kruppajo/work/GitHub/jkruppa.github.io/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{F091B0C2-8F25-3F41-ADE7-B65236A1C320}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{DB350A75-234B-5141-9148-AB877097AA5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1200" yWindow="880" windowWidth="31820" windowHeight="15660" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1520,8 +1520,8 @@
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W174"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I147" workbookViewId="0">
-      <selection activeCell="W174" sqref="W174"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="Z26" sqref="Z26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>